<commit_message>
Create update after 9/26/23 USST meeting
</commit_message>
<xml_diff>
--- a/Fall Flows 2023 Sept25 Draft.xlsx
+++ b/Fall Flows 2023 Sept25 Draft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/lelliott_usbr_gov/Documents/Documents/GitHub/Fall_Flow_Redd_Dewatering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C71633B-E44D-4C1D-9F12-735327A03421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C118A827-DA0D-4A86-AE9A-8FABD049065F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-21195" yWindow="2220" windowWidth="21600" windowHeight="11040" tabRatio="838" activeTab="5" xr2:uid="{8B6B0201-DD1B-4D0A-8FA2-1793C828B1EC}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" activeTab="5" xr2:uid="{8B6B0201-DD1B-4D0A-8FA2-1793C828B1EC}"/>
   </bookViews>
   <sheets>
     <sheet name="KES Flow all" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="128">
   <si>
     <t>Keswick Flows in cfs</t>
   </si>
@@ -497,9 +497,6 @@
     <t xml:space="preserve">  Alt 1b = Update of alternative 1a based on August 50% Exceedance as an updated template. Does not follow ramping rates. Developed on August 15, 2023.</t>
   </si>
   <si>
-    <t>Alt 1c = draft September 50% forecast. Developed 9/28/2023</t>
-  </si>
-  <si>
     <t>Alt 2a = Initial rough template scenario put together based on July 90% exceedance forecast. Does not follow ramping rates. Developed on 8/4/2023. Suggest eliminating from consideration because information is outdated.</t>
   </si>
   <si>
@@ -544,6 +541,18 @@
   <si>
     <t>Alt 3k = Developed to avoid dewatering winter-run redds while following operations goals described at 9/12/23 USST meeting (100-200 cfs drops per day, avoiding large drops expected to cause dewatering on days that the shallow redd monitoring crews cannot be in the field, holding at 5000 cfs over the winter)  and redd dewatering flows updated to use KES flows instead of KWK flows. Developed on 9/19/23.</t>
   </si>
+  <si>
+    <t>Alt 3l = Developed to reflect operations decisions made at 9/26/23 USST meeting (drop to 6400 cfs) and reflecting the possibility of returning to 6500 cfs in mid-October for rice decomp needs, and then ramping down to 5000 cfs in early November. Developed 9/26/23.</t>
+  </si>
+  <si>
+    <t>Alt 3m = Developed to reflect operations decisions made at 9/26/23 USST meeting (drop to 6400 cfs) but with further reductions to 6100 cfs, and reflecting the possibility of returning to 6500 cfs in mid-October for rice decomp needs, and then ramping down to 5000 cfs in early November. Developed 9/26/23.</t>
+  </si>
+  <si>
+    <t>Alt 1c = draft September 50% forecast. Developed 9/26/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alt 2E = draft September 90% forecast. Developed 9/13/23.  </t>
+  </si>
 </sst>
 </file>
 
@@ -553,7 +562,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -799,6 +808,13 @@
     </font>
     <font>
       <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -1611,7 +1627,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="215">
+  <cellXfs count="218">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2023,6 +2039,93 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2030,12 +2133,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2080,86 +2177,12 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="128">
@@ -39287,104 +39310,104 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="190" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="175" t="s">
+      <c r="B1" s="202" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="175" t="s">
+      <c r="C1" s="202" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="175" t="s">
+      <c r="D1" s="202" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="175" t="s">
+      <c r="E1" s="202" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="175" t="s">
+      <c r="F1" s="202" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="179" t="s">
+      <c r="G1" s="206" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="175" t="s">
+      <c r="H1" s="202" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="182" t="s">
+      <c r="I1" s="209" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="169" t="s">
+      <c r="J1" s="198" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="185" t="s">
+      <c r="K1" s="212" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="169" t="s">
+      <c r="L1" s="198" t="s">
         <v>64</v>
       </c>
       <c r="M1" s="168"/>
       <c r="N1" s="168"/>
-      <c r="O1" s="190" t="s">
+      <c r="O1" s="181" t="s">
         <v>53</v>
       </c>
-      <c r="P1" s="193" t="s">
+      <c r="P1" s="184" t="s">
         <v>65</v>
       </c>
-      <c r="Q1" s="194"/>
-      <c r="R1" s="194"/>
-      <c r="S1" s="194"/>
-      <c r="T1" s="194"/>
-      <c r="U1" s="194"/>
-      <c r="V1" s="194"/>
-      <c r="W1" s="194"/>
-      <c r="X1" s="194"/>
-      <c r="Y1" s="194"/>
-      <c r="Z1" s="194"/>
-      <c r="AA1" s="194"/>
-      <c r="AB1" s="194"/>
-      <c r="AC1" s="194"/>
-      <c r="AD1" s="194"/>
-      <c r="AE1" s="194"/>
-      <c r="AF1" s="194"/>
-      <c r="AG1" s="194"/>
-      <c r="AH1" s="194"/>
-      <c r="AI1" s="194"/>
-      <c r="AJ1" s="194"/>
-      <c r="AK1" s="194"/>
-      <c r="AL1" s="194"/>
-      <c r="AM1" s="194"/>
-      <c r="AN1" s="194"/>
-      <c r="AO1" s="194"/>
-      <c r="AP1" s="194"/>
-      <c r="AQ1" s="194"/>
-      <c r="AR1" s="194"/>
+      <c r="Q1" s="185"/>
+      <c r="R1" s="185"/>
+      <c r="S1" s="185"/>
+      <c r="T1" s="185"/>
+      <c r="U1" s="185"/>
+      <c r="V1" s="185"/>
+      <c r="W1" s="185"/>
+      <c r="X1" s="185"/>
+      <c r="Y1" s="185"/>
+      <c r="Z1" s="185"/>
+      <c r="AA1" s="185"/>
+      <c r="AB1" s="185"/>
+      <c r="AC1" s="185"/>
+      <c r="AD1" s="185"/>
+      <c r="AE1" s="185"/>
+      <c r="AF1" s="185"/>
+      <c r="AG1" s="185"/>
+      <c r="AH1" s="185"/>
+      <c r="AI1" s="185"/>
+      <c r="AJ1" s="185"/>
+      <c r="AK1" s="185"/>
+      <c r="AL1" s="185"/>
+      <c r="AM1" s="185"/>
+      <c r="AN1" s="185"/>
+      <c r="AO1" s="185"/>
+      <c r="AP1" s="185"/>
+      <c r="AQ1" s="185"/>
+      <c r="AR1" s="185"/>
       <c r="AS1" s="168"/>
       <c r="AT1" s="168"/>
       <c r="AU1" s="168"/>
       <c r="AV1" s="168"/>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A2" s="173"/>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="180"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="183"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="186"/>
-      <c r="L2" s="170"/>
+      <c r="A2" s="191"/>
+      <c r="B2" s="203"/>
+      <c r="C2" s="203"/>
+      <c r="D2" s="203"/>
+      <c r="E2" s="203"/>
+      <c r="F2" s="203"/>
+      <c r="G2" s="207"/>
+      <c r="H2" s="203"/>
+      <c r="I2" s="210"/>
+      <c r="J2" s="199"/>
+      <c r="K2" s="213"/>
+      <c r="L2" s="199"/>
       <c r="M2" s="168"/>
       <c r="N2" s="168"/>
-      <c r="O2" s="191"/>
-      <c r="P2" s="195" t="s">
+      <c r="O2" s="182"/>
+      <c r="P2" s="186" t="s">
         <v>66</v>
       </c>
-      <c r="Q2" s="196"/>
-      <c r="R2" s="172" t="s">
+      <c r="Q2" s="187"/>
+      <c r="R2" s="190" t="s">
         <v>67</v>
       </c>
       <c r="S2" s="82">
@@ -39477,24 +39500,24 @@
       <c r="AV2" s="168"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A3" s="173"/>
-      <c r="B3" s="176"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
-      <c r="F3" s="176"/>
-      <c r="G3" s="180"/>
-      <c r="H3" s="176"/>
-      <c r="I3" s="183"/>
-      <c r="J3" s="170"/>
-      <c r="K3" s="186"/>
-      <c r="L3" s="170"/>
+      <c r="A3" s="191"/>
+      <c r="B3" s="203"/>
+      <c r="C3" s="203"/>
+      <c r="D3" s="203"/>
+      <c r="E3" s="203"/>
+      <c r="F3" s="203"/>
+      <c r="G3" s="207"/>
+      <c r="H3" s="203"/>
+      <c r="I3" s="210"/>
+      <c r="J3" s="199"/>
+      <c r="K3" s="213"/>
+      <c r="L3" s="199"/>
       <c r="M3" s="168"/>
       <c r="N3" s="168"/>
-      <c r="O3" s="191"/>
-      <c r="P3" s="197"/>
-      <c r="Q3" s="198"/>
-      <c r="R3" s="173"/>
+      <c r="O3" s="182"/>
+      <c r="P3" s="188"/>
+      <c r="Q3" s="189"/>
+      <c r="R3" s="191"/>
       <c r="S3" s="88">
         <v>45069</v>
       </c>
@@ -39585,46 +39608,46 @@
       <c r="AV3" s="168"/>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A4" s="173"/>
-      <c r="B4" s="176"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="176"/>
-      <c r="F4" s="176"/>
-      <c r="G4" s="180"/>
-      <c r="H4" s="176"/>
-      <c r="I4" s="183"/>
-      <c r="J4" s="170"/>
-      <c r="K4" s="186"/>
-      <c r="L4" s="170"/>
+      <c r="A4" s="191"/>
+      <c r="B4" s="203"/>
+      <c r="C4" s="203"/>
+      <c r="D4" s="203"/>
+      <c r="E4" s="203"/>
+      <c r="F4" s="203"/>
+      <c r="G4" s="207"/>
+      <c r="H4" s="203"/>
+      <c r="I4" s="210"/>
+      <c r="J4" s="199"/>
+      <c r="K4" s="213"/>
+      <c r="L4" s="199"/>
       <c r="M4" s="168"/>
       <c r="N4" s="168"/>
-      <c r="O4" s="191"/>
-      <c r="P4" s="197"/>
-      <c r="Q4" s="198"/>
-      <c r="R4" s="173"/>
-      <c r="S4" s="199" t="s">
+      <c r="O4" s="182"/>
+      <c r="P4" s="188"/>
+      <c r="Q4" s="189"/>
+      <c r="R4" s="191"/>
+      <c r="S4" s="192" t="s">
         <v>68</v>
       </c>
-      <c r="T4" s="199"/>
-      <c r="U4" s="199"/>
-      <c r="V4" s="199"/>
-      <c r="W4" s="199"/>
-      <c r="X4" s="199"/>
-      <c r="Y4" s="199"/>
-      <c r="Z4" s="199"/>
-      <c r="AA4" s="199"/>
-      <c r="AB4" s="199"/>
-      <c r="AC4" s="199"/>
-      <c r="AD4" s="199"/>
-      <c r="AE4" s="199"/>
-      <c r="AF4" s="199"/>
-      <c r="AG4" s="199"/>
-      <c r="AH4" s="199"/>
-      <c r="AI4" s="199"/>
-      <c r="AJ4" s="199"/>
-      <c r="AK4" s="199"/>
-      <c r="AL4" s="199"/>
+      <c r="T4" s="192"/>
+      <c r="U4" s="192"/>
+      <c r="V4" s="192"/>
+      <c r="W4" s="192"/>
+      <c r="X4" s="192"/>
+      <c r="Y4" s="192"/>
+      <c r="Z4" s="192"/>
+      <c r="AA4" s="192"/>
+      <c r="AB4" s="192"/>
+      <c r="AC4" s="192"/>
+      <c r="AD4" s="192"/>
+      <c r="AE4" s="192"/>
+      <c r="AF4" s="192"/>
+      <c r="AG4" s="192"/>
+      <c r="AH4" s="192"/>
+      <c r="AI4" s="192"/>
+      <c r="AJ4" s="192"/>
+      <c r="AK4" s="192"/>
+      <c r="AL4" s="192"/>
       <c r="AM4" s="168"/>
       <c r="AN4" s="168"/>
       <c r="AO4" s="168"/>
@@ -39637,28 +39660,28 @@
       <c r="AV4" s="168"/>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A5" s="174"/>
-      <c r="B5" s="177"/>
-      <c r="C5" s="178"/>
-      <c r="D5" s="178"/>
-      <c r="E5" s="178"/>
-      <c r="F5" s="178"/>
-      <c r="G5" s="181"/>
-      <c r="H5" s="178"/>
-      <c r="I5" s="184"/>
-      <c r="J5" s="171"/>
-      <c r="K5" s="187"/>
-      <c r="L5" s="171"/>
+      <c r="A5" s="201"/>
+      <c r="B5" s="204"/>
+      <c r="C5" s="205"/>
+      <c r="D5" s="205"/>
+      <c r="E5" s="205"/>
+      <c r="F5" s="205"/>
+      <c r="G5" s="208"/>
+      <c r="H5" s="205"/>
+      <c r="I5" s="211"/>
+      <c r="J5" s="200"/>
+      <c r="K5" s="214"/>
+      <c r="L5" s="200"/>
       <c r="M5" s="168"/>
       <c r="N5" s="168"/>
-      <c r="O5" s="192"/>
+      <c r="O5" s="183"/>
       <c r="P5" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="Q5" s="196" t="s">
+      <c r="Q5" s="187" t="s">
         <v>70</v>
       </c>
-      <c r="R5" s="200"/>
+      <c r="R5" s="193"/>
       <c r="S5" s="96">
         <v>13000</v>
       </c>
@@ -39793,10 +39816,10 @@
       <c r="P6" s="110">
         <v>4001</v>
       </c>
-      <c r="Q6" s="201">
+      <c r="Q6" s="194">
         <v>15</v>
       </c>
-      <c r="R6" s="202"/>
+      <c r="R6" s="195"/>
       <c r="S6" s="111">
         <v>15</v>
       </c>
@@ -39935,10 +39958,10 @@
       <c r="P7" s="114">
         <v>4002</v>
       </c>
-      <c r="Q7" s="203">
+      <c r="Q7" s="196">
         <v>37</v>
       </c>
-      <c r="R7" s="204"/>
+      <c r="R7" s="197"/>
       <c r="S7" s="103" t="s">
         <v>47</v>
       </c>
@@ -40062,7 +40085,7 @@
       <c r="K8" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="L8" s="205" t="s">
+      <c r="L8" s="179" t="s">
         <v>76</v>
       </c>
       <c r="M8" s="113" t="s">
@@ -40077,10 +40100,10 @@
       <c r="P8" s="128">
         <v>4003</v>
       </c>
-      <c r="Q8" s="188">
+      <c r="Q8" s="172">
         <v>18</v>
       </c>
-      <c r="R8" s="189"/>
+      <c r="R8" s="173"/>
       <c r="S8" s="129" t="s">
         <v>47</v>
       </c>
@@ -40204,7 +40227,7 @@
       <c r="K9" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="L9" s="206"/>
+      <c r="L9" s="180"/>
       <c r="M9" s="113" t="s">
         <v>47</v>
       </c>
@@ -40217,10 +40240,10 @@
       <c r="P9" s="128">
         <v>4004</v>
       </c>
-      <c r="Q9" s="207">
+      <c r="Q9" s="170">
         <v>19</v>
       </c>
-      <c r="R9" s="208"/>
+      <c r="R9" s="171"/>
       <c r="S9" s="129" t="s">
         <v>47</v>
       </c>
@@ -40359,10 +40382,10 @@
       <c r="P10" s="128">
         <v>4005</v>
       </c>
-      <c r="Q10" s="188">
+      <c r="Q10" s="172">
         <v>17</v>
       </c>
-      <c r="R10" s="189"/>
+      <c r="R10" s="173"/>
       <c r="S10" s="129" t="s">
         <v>47</v>
       </c>
@@ -40501,10 +40524,10 @@
       <c r="P11" s="128">
         <v>4006</v>
       </c>
-      <c r="Q11" s="207">
+      <c r="Q11" s="170">
         <v>15</v>
       </c>
-      <c r="R11" s="208"/>
+      <c r="R11" s="171"/>
       <c r="S11" s="129" t="s">
         <v>47</v>
       </c>
@@ -40643,10 +40666,10 @@
       <c r="P12" s="128">
         <v>4007</v>
       </c>
-      <c r="Q12" s="188">
+      <c r="Q12" s="172">
         <v>54</v>
       </c>
-      <c r="R12" s="189"/>
+      <c r="R12" s="173"/>
       <c r="S12" s="129" t="s">
         <v>47</v>
       </c>
@@ -40785,10 +40808,10 @@
       <c r="P13" s="128">
         <v>4008</v>
       </c>
-      <c r="Q13" s="207">
+      <c r="Q13" s="170">
         <v>18</v>
       </c>
-      <c r="R13" s="208"/>
+      <c r="R13" s="171"/>
       <c r="S13" s="129" t="s">
         <v>47</v>
       </c>
@@ -40927,10 +40950,10 @@
       <c r="P14" s="128">
         <v>4009</v>
       </c>
-      <c r="Q14" s="188">
+      <c r="Q14" s="172">
         <v>13</v>
       </c>
-      <c r="R14" s="189"/>
+      <c r="R14" s="173"/>
       <c r="S14" s="129" t="s">
         <v>47</v>
       </c>
@@ -41036,7 +41059,7 @@
       <c r="E15" s="118">
         <v>12</v>
       </c>
-      <c r="F15" s="214"/>
+      <c r="F15" s="169"/>
       <c r="G15" s="122">
         <v>10673</v>
       </c>
@@ -41067,10 +41090,10 @@
       <c r="P15" s="128">
         <v>4010</v>
       </c>
-      <c r="Q15" s="207">
+      <c r="Q15" s="170">
         <v>12</v>
       </c>
-      <c r="R15" s="208"/>
+      <c r="R15" s="171"/>
       <c r="S15" s="129" t="s">
         <v>47</v>
       </c>
@@ -41211,10 +41234,10 @@
       <c r="P16" s="128">
         <v>4011</v>
       </c>
-      <c r="Q16" s="188">
+      <c r="Q16" s="172">
         <v>11</v>
       </c>
-      <c r="R16" s="189"/>
+      <c r="R16" s="173"/>
       <c r="S16" s="129" t="s">
         <v>47</v>
       </c>
@@ -41353,10 +41376,10 @@
       <c r="P17" s="128">
         <v>4012</v>
       </c>
-      <c r="Q17" s="207">
+      <c r="Q17" s="170">
         <v>17</v>
       </c>
-      <c r="R17" s="208"/>
+      <c r="R17" s="171"/>
       <c r="S17" s="129" t="s">
         <v>47</v>
       </c>
@@ -41495,10 +41518,10 @@
       <c r="P18" s="128">
         <v>4013</v>
       </c>
-      <c r="Q18" s="188">
+      <c r="Q18" s="172">
         <v>17</v>
       </c>
-      <c r="R18" s="189"/>
+      <c r="R18" s="173"/>
       <c r="S18" s="129" t="s">
         <v>47</v>
       </c>
@@ -41637,10 +41660,10 @@
       <c r="P19" s="128">
         <v>4014</v>
       </c>
-      <c r="Q19" s="207">
+      <c r="Q19" s="170">
         <v>24</v>
       </c>
-      <c r="R19" s="208"/>
+      <c r="R19" s="171"/>
       <c r="S19" s="129" t="s">
         <v>47</v>
       </c>
@@ -41779,10 +41802,10 @@
       <c r="P20" s="128">
         <v>4015</v>
       </c>
-      <c r="Q20" s="188">
+      <c r="Q20" s="172">
         <v>49</v>
       </c>
-      <c r="R20" s="189"/>
+      <c r="R20" s="173"/>
       <c r="S20" s="129" t="s">
         <v>47</v>
       </c>
@@ -41921,10 +41944,10 @@
       <c r="P21" s="128">
         <v>4016</v>
       </c>
-      <c r="Q21" s="207">
+      <c r="Q21" s="170">
         <v>34</v>
       </c>
-      <c r="R21" s="208"/>
+      <c r="R21" s="171"/>
       <c r="S21" s="129" t="s">
         <v>47</v>
       </c>
@@ -42063,10 +42086,10 @@
       <c r="P22" s="128">
         <v>4017</v>
       </c>
-      <c r="Q22" s="188">
+      <c r="Q22" s="172">
         <v>19</v>
       </c>
-      <c r="R22" s="189"/>
+      <c r="R22" s="173"/>
       <c r="S22" s="129" t="s">
         <v>47</v>
       </c>
@@ -42205,10 +42228,10 @@
       <c r="P23" s="128">
         <v>4018</v>
       </c>
-      <c r="Q23" s="207">
+      <c r="Q23" s="170">
         <v>26</v>
       </c>
-      <c r="R23" s="208"/>
+      <c r="R23" s="171"/>
       <c r="S23" s="129" t="s">
         <v>47</v>
       </c>
@@ -42347,10 +42370,10 @@
       <c r="P24" s="128">
         <v>4019</v>
       </c>
-      <c r="Q24" s="188">
+      <c r="Q24" s="172">
         <v>39</v>
       </c>
-      <c r="R24" s="189"/>
+      <c r="R24" s="173"/>
       <c r="S24" s="129" t="s">
         <v>47</v>
       </c>
@@ -42489,10 +42512,10 @@
       <c r="P25" s="128">
         <v>4020</v>
       </c>
-      <c r="Q25" s="207">
+      <c r="Q25" s="170">
         <v>35</v>
       </c>
-      <c r="R25" s="208"/>
+      <c r="R25" s="171"/>
       <c r="S25" s="129" t="s">
         <v>47</v>
       </c>
@@ -42631,10 +42654,10 @@
       <c r="P26" s="128">
         <v>4021</v>
       </c>
-      <c r="Q26" s="188">
+      <c r="Q26" s="172">
         <v>37</v>
       </c>
-      <c r="R26" s="189"/>
+      <c r="R26" s="173"/>
       <c r="S26" s="129" t="s">
         <v>47</v>
       </c>
@@ -42773,10 +42796,10 @@
       <c r="P27" s="128">
         <v>4022</v>
       </c>
-      <c r="Q27" s="207">
+      <c r="Q27" s="170">
         <v>32</v>
       </c>
-      <c r="R27" s="208"/>
+      <c r="R27" s="171"/>
       <c r="S27" s="129" t="s">
         <v>47</v>
       </c>
@@ -42915,10 +42938,10 @@
       <c r="P28" s="128">
         <v>4023</v>
       </c>
-      <c r="Q28" s="188">
+      <c r="Q28" s="172">
         <v>21</v>
       </c>
-      <c r="R28" s="189"/>
+      <c r="R28" s="173"/>
       <c r="S28" s="129" t="s">
         <v>47</v>
       </c>
@@ -43057,10 +43080,10 @@
       <c r="P29" s="128">
         <v>4024</v>
       </c>
-      <c r="Q29" s="207">
+      <c r="Q29" s="170">
         <v>18</v>
       </c>
-      <c r="R29" s="208"/>
+      <c r="R29" s="171"/>
       <c r="S29" s="129" t="s">
         <v>47</v>
       </c>
@@ -43166,7 +43189,7 @@
       <c r="E30" s="118">
         <v>10</v>
       </c>
-      <c r="F30" s="214"/>
+      <c r="F30" s="169"/>
       <c r="G30" s="122">
         <v>11128</v>
       </c>
@@ -43197,10 +43220,10 @@
       <c r="P30" s="128">
         <v>4025</v>
       </c>
-      <c r="Q30" s="188">
+      <c r="Q30" s="172">
         <v>10</v>
       </c>
-      <c r="R30" s="189"/>
+      <c r="R30" s="173"/>
       <c r="S30" s="129" t="s">
         <v>47</v>
       </c>
@@ -43341,10 +43364,10 @@
       <c r="P31" s="152">
         <v>4026</v>
       </c>
-      <c r="Q31" s="209">
+      <c r="Q31" s="174">
         <v>13</v>
       </c>
-      <c r="R31" s="210"/>
+      <c r="R31" s="175"/>
       <c r="S31" s="153" t="s">
         <v>47</v>
       </c>
@@ -45092,11 +45115,11 @@
       <c r="I64" s="168"/>
       <c r="J64" s="159"/>
       <c r="K64" s="168"/>
-      <c r="L64" s="211" t="s">
+      <c r="L64" s="176" t="s">
         <v>99</v>
       </c>
-      <c r="M64" s="211"/>
-      <c r="N64" s="211"/>
+      <c r="M64" s="176"/>
+      <c r="N64" s="176"/>
       <c r="O64" s="168"/>
       <c r="P64" s="168"/>
       <c r="Q64" s="168"/>
@@ -45144,9 +45167,9 @@
       <c r="I65" s="168"/>
       <c r="J65" s="159"/>
       <c r="K65" s="168"/>
-      <c r="L65" s="212"/>
-      <c r="M65" s="212"/>
-      <c r="N65" s="212"/>
+      <c r="L65" s="177"/>
+      <c r="M65" s="177"/>
+      <c r="N65" s="177"/>
       <c r="O65" s="168"/>
       <c r="P65" s="168"/>
       <c r="Q65" s="168"/>
@@ -45194,9 +45217,9 @@
       <c r="I66" s="168"/>
       <c r="J66" s="159"/>
       <c r="K66" s="168"/>
-      <c r="L66" s="212"/>
-      <c r="M66" s="212"/>
-      <c r="N66" s="212"/>
+      <c r="L66" s="177"/>
+      <c r="M66" s="177"/>
+      <c r="N66" s="177"/>
       <c r="O66" s="168"/>
       <c r="P66" s="168"/>
       <c r="Q66" s="168"/>
@@ -45244,9 +45267,9 @@
       <c r="I67" s="168"/>
       <c r="J67" s="159"/>
       <c r="K67" s="168"/>
-      <c r="L67" s="212"/>
-      <c r="M67" s="212"/>
-      <c r="N67" s="212"/>
+      <c r="L67" s="177"/>
+      <c r="M67" s="177"/>
+      <c r="N67" s="177"/>
       <c r="O67" s="168"/>
       <c r="P67" s="168"/>
       <c r="Q67" s="168"/>
@@ -45294,9 +45317,9 @@
       <c r="I68" s="168"/>
       <c r="J68" s="159"/>
       <c r="K68" s="168"/>
-      <c r="L68" s="213"/>
-      <c r="M68" s="213"/>
-      <c r="N68" s="213"/>
+      <c r="L68" s="178"/>
+      <c r="M68" s="178"/>
+      <c r="N68" s="178"/>
       <c r="O68" s="168"/>
       <c r="P68" s="168"/>
       <c r="Q68" s="168"/>
@@ -45484,16 +45507,26 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="L64:N68"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="L1:L5"/>
+    <mergeCell ref="A1:A5"/>
+    <mergeCell ref="B1:B5"/>
+    <mergeCell ref="C1:C5"/>
+    <mergeCell ref="D1:D5"/>
+    <mergeCell ref="E1:E5"/>
+    <mergeCell ref="F1:F5"/>
+    <mergeCell ref="G1:G5"/>
+    <mergeCell ref="H1:H5"/>
+    <mergeCell ref="I1:I5"/>
+    <mergeCell ref="J1:J5"/>
+    <mergeCell ref="K1:K5"/>
+    <mergeCell ref="O1:O5"/>
+    <mergeCell ref="P1:AR1"/>
+    <mergeCell ref="P2:Q4"/>
+    <mergeCell ref="R2:R4"/>
+    <mergeCell ref="S4:AL4"/>
+    <mergeCell ref="Q5:R5"/>
     <mergeCell ref="L8:L9"/>
     <mergeCell ref="Q8:R8"/>
     <mergeCell ref="Q9:R9"/>
@@ -45510,26 +45543,16 @@
     <mergeCell ref="Q20:R20"/>
     <mergeCell ref="Q21:R21"/>
     <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="O1:O5"/>
-    <mergeCell ref="P1:AR1"/>
-    <mergeCell ref="P2:Q4"/>
-    <mergeCell ref="R2:R4"/>
-    <mergeCell ref="S4:AL4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="L1:L5"/>
-    <mergeCell ref="A1:A5"/>
-    <mergeCell ref="B1:B5"/>
-    <mergeCell ref="C1:C5"/>
-    <mergeCell ref="D1:D5"/>
-    <mergeCell ref="E1:E5"/>
-    <mergeCell ref="F1:F5"/>
-    <mergeCell ref="G1:G5"/>
-    <mergeCell ref="H1:H5"/>
-    <mergeCell ref="I1:I5"/>
-    <mergeCell ref="J1:J5"/>
-    <mergeCell ref="K1:K5"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="L64:N68"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q28:R28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -45552,10 +45575,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA370860-48CD-4B92-B790-82066B2C7AEE}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45624,11 +45647,11 @@
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="B12" s="3"/>
+    <row r="12" spans="1:2" s="39" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="216" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="217"/>
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
@@ -45636,85 +45659,101 @@
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:2" s="25" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B16" s="5"/>
     </row>
     <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B17" s="5"/>
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="3"/>
+      <c r="A18" s="216" t="s">
+        <v>127</v>
+      </c>
+      <c r="B18" s="5"/>
     </row>
     <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>114</v>
-      </c>
+      <c r="A19" s="13"/>
+      <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
-        <v>117</v>
+    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
-        <v>119</v>
+      <c r="A24" s="17" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="39" t="s">
-        <v>120</v>
+      <c r="A25" s="25" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="39" t="s">
-        <v>121</v>
+      <c r="A26" s="25" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="39" t="s">
-        <v>122</v>
+      <c r="A27" s="25" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="39" t="s">
-        <v>123</v>
+      <c r="A28" s="25" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="215" t="s">
         <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="215" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>